<commit_message>
refactoring test data for schema changes
</commit_message>
<xml_diff>
--- a/protected/data/master/issue.xlsx
+++ b/protected/data/master/issue.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="96" windowWidth="19140" windowHeight="9264"/>
+    <workbookView xWindow="96" yWindow="96" windowWidth="19140" windowHeight="9264" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="issue" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>id</t>
   </si>
@@ -63,15 +63,6 @@
     <t>Incorrect PCB layout</t>
   </si>
   <si>
-    <t>TYPE3</t>
-  </si>
-  <si>
-    <t>TYPE2</t>
-  </si>
-  <si>
-    <t>TYPE1</t>
-  </si>
-  <si>
     <t>Issue is active.</t>
   </si>
   <si>
@@ -97,6 +88,24 @@
   </si>
   <si>
     <t>requestor_id</t>
+  </si>
+  <si>
+    <t>BUG</t>
+  </si>
+  <si>
+    <t>FEATURE</t>
+  </si>
+  <si>
+    <t>TASK</t>
+  </si>
+  <si>
+    <t>An activity.</t>
+  </si>
+  <si>
+    <t>An observation of a deficiency in behavior compared to requirements.</t>
+  </si>
+  <si>
+    <t>A behavior to be considered for requirement.</t>
   </si>
 </sst>
 </file>
@@ -996,7 +1005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1036,7 +1045,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>6</v>
@@ -1068,7 +1077,7 @@
         <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2" s="2">
         <v>3</v>
@@ -1111,7 +1120,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2">
         <v>3</v>
@@ -1151,10 +1160,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2">
         <v>6</v>
@@ -1199,7 +1208,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1225,10 +1236,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1236,10 +1247,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1256,11 +1267,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.5546875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="2.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52" style="4" customWidth="1"/>
     <col min="4" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
@@ -1275,15 +1288,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1291,10 +1304,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1302,10 +1315,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor activity into issue
</commit_message>
<xml_diff>
--- a/protected/data/master/issue.xlsx
+++ b/protected/data/master/issue.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="96" windowWidth="19140" windowHeight="9264" activeTab="2"/>
+    <workbookView xWindow="96" yWindow="96" windowWidth="19140" windowHeight="9264"/>
   </bookViews>
   <sheets>
     <sheet name="issue" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>id</t>
   </si>
@@ -63,18 +63,6 @@
     <t>Incorrect PCB layout</t>
   </si>
   <si>
-    <t>Issue is active.</t>
-  </si>
-  <si>
-    <t>ACTIVE</t>
-  </si>
-  <si>
-    <t>Issue is closed.</t>
-  </si>
-  <si>
-    <t>INACTIVE</t>
-  </si>
-  <si>
     <t>Connectivity of PCB-type inductor is incorrect.</t>
   </si>
   <si>
@@ -99,13 +87,40 @@
     <t>TASK</t>
   </si>
   <si>
-    <t>An activity.</t>
-  </si>
-  <si>
-    <t>An observation of a deficiency in behavior compared to requirements.</t>
-  </si>
-  <si>
-    <t>A behavior to be considered for requirement.</t>
+    <t>type</t>
+  </si>
+  <si>
+    <t>NOT STARTED</t>
+  </si>
+  <si>
+    <t>STARTED</t>
+  </si>
+  <si>
+    <t>FINISHED</t>
+  </si>
+  <si>
+    <t>Issue has not been started</t>
+  </si>
+  <si>
+    <t>Issue has been started</t>
+  </si>
+  <si>
+    <t>Issue has been finished (resolved)</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>Deficiency in behavior compared to requirements.</t>
+  </si>
+  <si>
+    <t>Desired behavior, but not required.</t>
+  </si>
+  <si>
+    <t>Activity requiring effort to resolve (neither bug or feature)</t>
+  </si>
+  <si>
+    <t>status</t>
   </si>
 </sst>
 </file>
@@ -1005,7 +1020,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1045,7 +1060,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>6</v>
@@ -1077,7 +1092,7 @@
         <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D2" s="2">
         <v>3</v>
@@ -1086,7 +1101,7 @@
         <v>15</v>
       </c>
       <c r="F2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2" s="2">
         <v>3</v>
@@ -1095,7 +1110,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" s="1">
         <v>41899</v>
@@ -1120,7 +1135,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2">
         <v>3</v>
@@ -1129,13 +1144,13 @@
         <v>1</v>
       </c>
       <c r="F3" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3" s="2">
         <v>3</v>
       </c>
       <c r="H3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3" s="2">
         <v>1</v>
@@ -1160,22 +1175,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2">
         <v>6</v>
       </c>
       <c r="F4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4" s="2">
         <v>6</v>
       </c>
       <c r="H4" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J4" s="2">
         <v>1</v>
@@ -1206,56 +1221,73 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6" style="4" customWidth="1"/>
-    <col min="2" max="2" width="8.77734375" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" style="4" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="2" width="5.77734375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" style="8" customWidth="1"/>
+    <col min="4" max="4" width="55.77734375" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>17</v>
+      <c r="B2" s="7">
+        <v>0</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>15</v>
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="C4" s="5"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7">
+        <v>2</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.39410000000000006" bottom="0.39410000000000006" header="0" footer="0"/>
@@ -1265,60 +1297,72 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52" style="4" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="2" width="5.77734375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="55.77734375" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>28</v>
+      <c r="B2" s="7">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>29</v>
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>27</v>
+      <c r="B4" s="7">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>